<commit_message>
New progs Commit on 30May
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>TestCase</t>
   </si>
@@ -53,12 +53,19 @@
   </si>
   <si>
     <t>Kumar</t>
+  </si>
+  <si>
+    <t>C:\Users\mkhedkar\eclipse-workspace\CGPracticeProject\TestData.xlsx</t>
+  </si>
+  <si>
+    <t>MKtest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -399,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
@@ -428,6 +435,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -438,6 +448,9 @@
       </c>
       <c r="C3" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>